<commit_message>
Added the code for PID and rotation checklist
</commit_message>
<xml_diff>
--- a/Updated PID.xlsx
+++ b/Updated PID.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yewheng/Desktop/CZ3004-MDP-Arduino/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielwijaya19/Desktop/Arduino-Explorer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF893BBA-F7A8-7340-9EA8-5E593E3FFD16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD438C5-A3D5-A34B-8D78-F1BDADFA11F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16300" windowHeight="16200" xr2:uid="{5602EDE8-970A-B14A-AEE3-714A8B5C1797}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{5602EDE8-970A-B14A-AEE3-714A8B5C1797}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -156,17 +156,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2367,8 +2367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271AA3A8-5A4A-6D4B-A421-65B6ADB34D30}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2517,303 +2517,303 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="D30" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2">
         <v>0.1</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0.08</v>
-      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="2">
         <v>0.02</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="2">
         <v>0.02</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="2">
         <f xml:space="preserve"> B32 + (B30/2)</f>
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="C33" s="2" t="s">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <f xml:space="preserve"> D32 + (D30/2)</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="4">
-        <v>52.91</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="2">
+        <v>70.91</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="4">
-        <v>59.95</v>
+      <c r="D34" s="2">
+        <v>77.67</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="4">
-        <v>61.22</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="2">
+        <v>87.98</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="4">
-        <v>68.849999999999994</v>
+      <c r="D35" s="2">
+        <v>95.28</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="2">
         <v>250</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
         <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="2">
         <v>300</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="2">
         <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="2">
         <f xml:space="preserve"> (B35 - B34) / (B37 - B36)</f>
-        <v>0.16620000000000004</v>
-      </c>
-      <c r="C39" s="2" t="s">
+        <v>0.34140000000000015</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="2">
         <f xml:space="preserve"> (D35 - D34) / (D37 - D36)</f>
-        <v>0.17799999999999983</v>
+        <v>0.35220000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="2">
         <f xml:space="preserve"> (1.2 * B31) / (B39 * B33)</f>
-        <v>32.089851584436417</v>
-      </c>
-      <c r="C40" s="2" t="s">
+        <v>9.3731693028705276</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="2">
         <f xml:space="preserve"> (1.2 * D31) / (D39 * D33)</f>
-        <v>23.970037453183547</v>
+        <v>7.5714556123414729</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="2">
         <f>(0.6*B31)/(B39*(B33^2))</f>
-        <v>713.10781298747588</v>
-      </c>
-      <c r="C41" s="2" t="s">
+        <v>104.14632558745032</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="2">
         <f>(0.6*D31)/(D39*(D33^2))</f>
-        <v>532.66749895963437</v>
+        <v>84.127284581571914</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="2">
         <f xml:space="preserve"> (0.6 * B31) / B39</f>
-        <v>0.36101083032490966</v>
-      </c>
-      <c r="C42" s="2" t="s">
+        <v>0.21089630931458689</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="2">
         <f xml:space="preserve"> (0.6 * D31) / D39</f>
-        <v>0.26966292134831488</v>
+        <v>0.17035775127768313</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="2">
         <f>B40</f>
-        <v>32.089851584436417</v>
-      </c>
-      <c r="C44" s="2" t="s">
+        <v>9.3731693028705276</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="2">
         <f>D40</f>
-        <v>23.970037453183547</v>
+        <v>7.5714556123414729</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="2">
         <f xml:space="preserve"> B41 * B30</f>
-        <v>3.5655390649373793</v>
-      </c>
-      <c r="C45" s="2" t="s">
+        <v>5.2073162793725167</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="2">
         <f xml:space="preserve"> D41 * D30</f>
-        <v>2.6633374947981721</v>
+        <v>4.2063642290785959</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="2">
         <f xml:space="preserve"> B42 / B30</f>
-        <v>72.202166064981924</v>
-      </c>
-      <c r="C46" s="2" t="s">
+        <v>4.2179261862917379</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="2">
         <f xml:space="preserve"> D42 / D30</f>
-        <v>53.932584269662975</v>
+        <v>3.4071550255536622</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="2">
         <f xml:space="preserve"> B44 + B45 + B46</f>
-        <v>107.85755671435572</v>
-      </c>
-      <c r="C47" s="2" t="s">
+        <v>18.798411768534784</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="2">
         <f xml:space="preserve"> D44 + D45 + D46</f>
-        <v>80.565959217644689</v>
+        <v>15.184974866973731</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="2">
         <f xml:space="preserve"> B44 - (2 * B46)</f>
-        <v>-112.31448054552743</v>
-      </c>
-      <c r="C48" s="2" t="s">
+        <v>0.93731693028705187</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="2">
         <f xml:space="preserve"> D44 - (2 * D46)</f>
-        <v>-83.895131086142399</v>
+        <v>0.75714556123414845</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="2">
         <f xml:space="preserve"> B46</f>
-        <v>72.202166064981924</v>
-      </c>
-      <c r="C49" s="2" t="s">
+        <v>4.2179261862917379</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="2">
         <f xml:space="preserve"> D46</f>
-        <v>53.932584269662975</v>
+        <v>3.4071550255536622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>